<commit_message>
improve modularity for juvenile/adult selection
</commit_message>
<xml_diff>
--- a/Lm_included.xlsx
+++ b/Lm_included.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="58">
   <si>
     <t>nm</t>
   </si>
@@ -178,16 +178,22 @@
     <t>Sebastes norvegicus</t>
   </si>
   <si>
-    <t>50 % Size at Maturity (cm)</t>
-  </si>
-  <si>
-    <t>BTS #</t>
-  </si>
-  <si>
     <t>Common Name</t>
   </si>
   <si>
     <t>Taxon</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>SVSPP</t>
+  </si>
+  <si>
+    <t>Lm</t>
   </si>
 </sst>
 </file>
@@ -1018,7 +1024,7 @@
   <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1027,27 +1033,33 @@
     <col min="3" max="3" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="14" width="9.140625" style="3"/>
+    <col min="8" max="14" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G1" t="s">
         <v>55</v>
       </c>
-      <c r="C1" t="s">
-        <v>54</v>
-      </c>
-      <c r="D1" t="s">
-        <v>53</v>
-      </c>
-      <c r="E1" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>38</v>
       </c>
@@ -1064,7 +1076,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
@@ -1080,8 +1092,14 @@
       <c r="E3">
         <v>43</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="G3">
+        <v>3.08</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>16</v>
       </c>
@@ -1097,8 +1115,14 @@
       <c r="E4">
         <v>36</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="G4">
+        <v>3.13</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>10</v>
       </c>
@@ -1115,7 +1139,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>23</v>
       </c>
@@ -1132,7 +1156,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>47</v>
       </c>
@@ -1149,7 +1173,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -1166,7 +1190,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>1</v>
       </c>
@@ -1183,7 +1207,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -1200,7 +1224,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>35</v>
       </c>
@@ -1217,7 +1241,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>29</v>
       </c>
@@ -1234,7 +1258,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>32</v>
       </c>
@@ -1251,7 +1275,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>26</v>
       </c>
@@ -1268,7 +1292,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="3" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -1284,8 +1308,10 @@
       <c r="E15" s="2">
         <v>16</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15"/>
+      <c r="G15"/>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>13</v>
       </c>
@@ -1302,7 +1328,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>19</v>
       </c>
@@ -1319,7 +1345,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>44</v>
       </c>
@@ -1336,7 +1362,10 @@
         <v>37</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="3" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="19" spans="1:7" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="F19"/>
+      <c r="G19"/>
+    </row>
   </sheetData>
   <sortState ref="A2:F19">
     <sortCondition ref="D2:D19"/>

</xml_diff>